<commit_message>
Updated typo error in weatherfiles_stations_1009.csv
</commit_message>
<xml_diff>
--- a/iso_simulator/annualSimulation/LCA/Primary_energy_and_emission_factors.xlsx
+++ b/iso_simulator/annualSimulation/LCA/Primary_energy_and_emission_factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tudublin-my.sharepoint.com/personal/d17128779_mytudublin_ie/Documents/GitHub/DIBS---Dynamic-ISO-Building-Simulator/iso_simulator/annualSimulation/LCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{39144B03-9582-4C0A-9967-1057809B5CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3C7F3E2-B437-47DC-A849-23E15998380B}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{39144B03-9582-4C0A-9967-1057809B5CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A99778A-96D8-409B-8C26-4FE559F77731}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary_energy_and_emission_fac" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="84">
   <si>
     <t>Rote Werte sind nicht GEG konform und müssen entsprechend § 22 bzw. § 85 nach DIN V 18599-9:2018-09 ermittelt werden!</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>and Electriciy grid mix use and small losses (therefore smaler COP)</t>
+  </si>
+  <si>
+    <t>German building energy act (GEG 2020)</t>
   </si>
 </sst>
 </file>
@@ -743,6 +746,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -760,10 +767,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -781,6 +784,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1049,7 +1056,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,6 +1102,9 @@
       <c r="E2" s="42" t="s">
         <v>62</v>
       </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
@@ -1599,7 +1609,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="65" t="s">
+      <c r="A32" s="59" t="s">
         <v>72</v>
       </c>
       <c r="B32" s="50">
@@ -1619,7 +1629,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="60" t="s">
         <v>79</v>
       </c>
       <c r="B33" s="57">
@@ -1650,7 +1660,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="59" t="s">
         <v>71</v>
       </c>
       <c r="B34" s="50">
@@ -2492,7 +2502,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="61" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2524,7 +2534,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
+      <c r="A3" s="62"/>
       <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
@@ -2554,7 +2564,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="60"/>
+      <c r="A4" s="62"/>
       <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
@@ -2584,7 +2594,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
@@ -2614,7 +2624,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
+      <c r="A6" s="62"/>
       <c r="B6" s="19" t="s">
         <v>7</v>
       </c>
@@ -2644,7 +2654,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="60"/>
+      <c r="A7" s="62"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -2674,7 +2684,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -2704,7 +2714,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="12" t="s">
         <v>10</v>
       </c>
@@ -2734,7 +2744,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="60"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="12" t="s">
         <v>11</v>
       </c>
@@ -2764,7 +2774,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="60"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="12" t="s">
         <v>12</v>
       </c>
@@ -2794,7 +2804,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="60"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="12" t="s">
         <v>13</v>
       </c>
@@ -2824,7 +2834,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="60"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="19" t="s">
         <v>14</v>
       </c>
@@ -2854,7 +2864,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="32" t="s">
         <v>15</v>
       </c>
@@ -2884,7 +2894,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="60"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="32" t="s">
         <v>16</v>
       </c>
@@ -2914,7 +2924,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="36" t="s">
         <v>17</v>
       </c>
@@ -2944,7 +2954,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="60"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="32" t="s">
         <v>18</v>
       </c>
@@ -2974,7 +2984,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="60"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="32" t="s">
         <v>19</v>
       </c>
@@ -3004,7 +3014,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="60"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="36" t="s">
         <v>20</v>
       </c>
@@ -3034,7 +3044,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="60"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="12" t="s">
         <v>21</v>
       </c>
@@ -3064,7 +3074,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="60"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="12" t="s">
         <v>22</v>
       </c>
@@ -3094,7 +3104,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="60"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="12" t="s">
         <v>23</v>
       </c>
@@ -3124,7 +3134,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="60"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="19" t="s">
         <v>24</v>
       </c>
@@ -3154,7 +3164,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="60"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="12" t="s">
         <v>25</v>
       </c>
@@ -3184,7 +3194,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="60"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="32" t="s">
         <v>26</v>
       </c>
@@ -3214,7 +3224,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="61"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="19" t="s">
         <v>27</v>
       </c>
@@ -3244,7 +3254,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="62" t="s">
+      <c r="A27" s="64" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -3276,7 +3286,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="63"/>
+      <c r="A28" s="65"/>
       <c r="B28" s="12" t="s">
         <v>30</v>
       </c>
@@ -3306,7 +3316,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="64"/>
+      <c r="A29" s="66"/>
       <c r="B29" s="19" t="s">
         <v>31</v>
       </c>

</xml_diff>